<commit_message>
Fix request config file of transit line filter integration test
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D72DF6-D413-41FE-A52B-A893A5BBE692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3A6284-89FA-40F4-A4F5-92629D7BAD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" activeTab="4" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
   <si>
     <t>location_id</t>
   </si>
@@ -55,9 +55,6 @@
     <t>capacity</t>
   </si>
   <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
     <t>tracks</t>
   </si>
   <si>
@@ -280,55 +277,16 @@
     <t>kelheim-v3.0-25pct</t>
   </si>
   <si>
-    <t>Bus_veh_type</t>
-  </si>
-  <si>
     <t>RE_RB_veh_type</t>
   </si>
   <si>
-    <t>regio_141134</t>
-  </si>
-  <si>
-    <t>regio_166759</t>
-  </si>
-  <si>
     <t>regio_314854</t>
   </si>
   <si>
-    <t>regio_215502</t>
-  </si>
-  <si>
-    <t>short_1119</t>
-  </si>
-  <si>
-    <t>short_6474</t>
-  </si>
-  <si>
-    <t>short_5972</t>
-  </si>
-  <si>
-    <t>short_9804</t>
-  </si>
-  <si>
     <t>regio_145538</t>
   </si>
   <si>
-    <t>regio_147682</t>
-  </si>
-  <si>
-    <t>regio_151384</t>
-  </si>
-  <si>
     <t>regio_172317</t>
-  </si>
-  <si>
-    <t>regio_293170</t>
-  </si>
-  <si>
-    <t>short_3740</t>
-  </si>
-  <si>
-    <t>short_6900</t>
   </si>
   <si>
     <t>deadHeadTripBeelineDistanceFactor</t>
@@ -760,428 +718,428 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.15234375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.84375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="6.4609375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="129.4609375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.81640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="6.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="129.453125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C4" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="7" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="C7" s="7">
         <v>0.25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="7">
         <f>90 / 3.6</f>
         <v>25</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C12" s="7">
         <f>15 * 60</f>
         <v>900</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>999</v>
       </c>
       <c r="D13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="E14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="C15" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C16" s="7">
         <v>3</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C17" s="7">
         <v>60</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C18" s="7">
         <f>2 * 60</f>
         <v>120</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
         <f>3 * 60</f>
         <v>180</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="7">
         <f>15000 * 1000</f>
         <v>15000000</v>
       </c>
       <c r="D20" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E20" s="3" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="C21" s="7">
         <v>100</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7">
         <v>25</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="7">
         <v>50</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="7">
         <v>75</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="7">
         <v>200</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1193,75 +1151,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD93A37-F36A-42AD-A931-6034D2325BC9}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.4609375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.23046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>600</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3">
-        <v>600</v>
-      </c>
-      <c r="D3">
-        <v>500</v>
-      </c>
-      <c r="E3">
         <v>2</v>
       </c>
     </row>
@@ -1274,33 +1215,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E31C2-14D1-4EB0-9548-0D6A0EA80330}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1310,61 +1251,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455315F6-EE05-465E-98C9-4563FB409249}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1374,21 +1280,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{319C589F-C9B8-4390-8C65-9522706FCF68}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="7.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1399,138 +1305,28 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13">
         <v>10</v>
       </c>
     </row>
@@ -1541,37 +1337,37 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A01B7B07-7F3C-4799-BD75-429B5670A61E}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.15234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1583,9 +1379,9 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1594,202 +1390,6 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="D3" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16">
-        <v>4</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D17" s="1">
         <v>0.66666666666666663</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ensure all allocated vehicle types in transit line sheet exist in the vehicle type sheet
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B3A6284-89FA-40F4-A4F5-92629D7BAD7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C3FA5-F115-4F54-B6EF-7B2BE770A84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -1153,20 +1153,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD93A37-F36A-42AD-A931-6034D2325BC9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.90625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="50.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="50.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E31C2-14D1-4EB0-9548-0D6A0EA80330}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rename integration test cases in request config files
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C3FA5-F115-4F54-B6EF-7B2BE770A84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40FFC7-31F8-4532-8624-FCD811397FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -277,9 +277,6 @@
     <t>kelheim-v3.0-25pct</t>
   </si>
   <si>
-    <t>RE_RB_veh_type</t>
-  </si>
-  <si>
     <t>regio_314854</t>
   </si>
   <si>
@@ -295,9 +292,6 @@
     <t>The factor that is applied to travel the beeline distance at speed limit, if no path in the network is found for the dead head trip between two locations.</t>
   </si>
   <si>
-    <t>it_config</t>
-  </si>
-  <si>
     <t>EPSG:25832</t>
   </si>
   <si>
@@ -317,6 +311,12 @@
   </si>
   <si>
     <t>regio_6022---2460</t>
+  </si>
+  <si>
+    <t>NEW_TYPE_NOT_EXISTING_IN_MATSIM</t>
+  </si>
+  <si>
+    <t>it_config_transit_line_filter</t>
   </si>
 </sst>
 </file>
@@ -718,9 +718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -757,7 +757,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
@@ -811,13 +811,13 @@
         <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,13 +860,13 @@
         <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C9" s="7">
         <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1153,15 +1153,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD93A37-F36A-42AD-A931-6034D2325BC9}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.90625" bestFit="1" customWidth="1"/>
@@ -1194,7 +1194,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C2">
         <v>600</v>
@@ -1215,33 +1215,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E31C2-14D1-4EB0-9548-0D6A0EA80330}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1270,7 +1270,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1284,13 +1284,13 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="36.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1310,10 +1310,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1321,10 +1321,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -1367,7 +1367,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3">
         <v>2</v>

</xml_diff>

<commit_message>
Remove CRS definition from pipeline
- Read files directly instead of using scenario utils.
- CRS from file is taken directly.
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40FFC7-31F8-4532-8624-FCD811397FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98ADDF2-E38E-4505-ABE1-70D972120097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario_info" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="maintenance_slots" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
   <si>
     <t>location_id</t>
   </si>
@@ -290,15 +290,6 @@
   </si>
   <si>
     <t>The factor that is applied to travel the beeline distance at speed limit, if no path in the network is found for the dead head trip between two locations.</t>
-  </si>
-  <si>
-    <t>EPSG:25832</t>
-  </si>
-  <si>
-    <t>networkCrs</t>
-  </si>
-  <si>
-    <t>The coordinate reference system of the network</t>
   </si>
   <si>
     <t>transit_line_id</t>
@@ -716,11 +707,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -757,7 +748,7 @@
         <v>71</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="3" t="s">
@@ -811,13 +802,16 @@
         <v>32</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>82</v>
+        <v>26</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -825,16 +819,17 @@
         <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C7" s="7">
-        <v>0.25</v>
+        <f>90 / 3.6</f>
+        <v>25</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -842,17 +837,13 @@
         <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C8" s="7">
-        <f>90 / 3.6</f>
-        <v>25</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,13 +851,16 @@
         <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="7">
-        <v>5</v>
+        <v>16</v>
+      </c>
+      <c r="C9" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -874,16 +868,16 @@
         <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="7" t="b">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -891,34 +885,34 @@
         <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="7">
-        <v>0</v>
+        <f>15 * 60</f>
+        <v>900</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7">
-        <f>15 * 60</f>
-        <v>900</v>
+        <v>999</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -926,16 +920,13 @@
         <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="7">
-        <v>999</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -943,30 +934,33 @@
         <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="C14" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="7" t="b">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C15" s="7">
+        <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -974,16 +968,16 @@
         <v>43</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C16" s="7">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -991,16 +985,17 @@
         <v>43</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7">
-        <v>60</v>
+        <f>2 * 60</f>
+        <v>120</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1008,53 +1003,52 @@
         <v>43</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" s="7">
-        <f>2 * 60</f>
-        <v>120</v>
+        <f>3 * 60</f>
+        <v>180</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="7">
-        <f>3 * 60</f>
-        <v>180</v>
+        <f>15000 * 1000</f>
+        <v>15000000</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="7">
-        <f>15000 * 1000</f>
-        <v>15000000</v>
+        <v>100</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1062,16 +1056,16 @@
         <v>9</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C21" s="7">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1079,16 +1073,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" s="7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1096,16 +1090,16 @@
         <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" s="7">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1113,37 +1107,20 @@
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C24" s="7">
-        <v>75</v>
+        <v>200</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="7">
-        <v>200</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="3" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E25" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
+  <autoFilter ref="A1:E24" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1194,7 +1171,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>600</v>
@@ -1216,32 +1193,33 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1291,7 @@
         <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -1324,7 +1302,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>10</v>

</xml_diff>

<commit_message>
Introduce capacity factor to reflect some buffer when planing for given demand
</commit_message>
<xml_diff>
--- a/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
+++ b/integration-test/input/de/kelheim/kelheim-v3.0/25pct/kelheim-v3.0-25pct.rssched_request_config_transit_line_filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devsbb\code\github\rssched\rssched-matsim-client\integration-test\input\de\kelheim\kelheim-v3.0\25pct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98ADDF2-E38E-4505-ABE1-70D972120097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACF7321C-84F5-4B08-B863-AD95D13D8B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{DC1F9231-C487-4AC9-83CB-859BC56E9E26}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="maintenance_slots" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">scenario_info!$A$1:$E$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="93">
   <si>
     <t>location_id</t>
   </si>
@@ -308,6 +308,21 @@
   </si>
   <si>
     <t>it_config_transit_line_filter</t>
+  </si>
+  <si>
+    <t>deadHeadTripAllowedModes</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>Deadhead trips are routed using network links that match one of these allowed modes (list sperated with colon: pt,rail)</t>
+  </si>
+  <si>
+    <t>capacityFactor</t>
+  </si>
+  <si>
+    <t>Adjust the passenger capacity of units to reflect deviations in passenger demand.</t>
   </si>
 </sst>
 </file>
@@ -707,11 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -819,17 +834,13 @@
         <v>32</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7">
-        <f>90 / 3.6</f>
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -837,13 +848,17 @@
         <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7">
-        <v>5</v>
+        <f>90 / 3.6</f>
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -851,16 +866,13 @@
         <v>32</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="C9" s="7">
+        <v>5</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -868,16 +880,16 @@
         <v>32</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="7">
+        <v>16</v>
+      </c>
+      <c r="C10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -885,48 +897,48 @@
         <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.33</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C13" s="7">
         <f>15 * 60</f>
         <v>900</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="7">
-        <v>999</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -934,50 +946,47 @@
         <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="7" t="b">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="C14" s="7">
+        <v>999</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="7">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="7">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -985,17 +994,16 @@
         <v>43</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C17" s="7">
-        <f>2 * 60</f>
-        <v>120</v>
+        <v>3</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1003,69 +1011,70 @@
         <v>43</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="7">
+        <v>60</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="7">
+        <f>2 * 60</f>
+        <v>120</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C20" s="7">
         <f>3 * 60</f>
         <v>180</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C21" s="7">
         <f>15000 * 1000</f>
         <v>15000000</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="7">
-        <v>100</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="7">
-        <v>25</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1073,16 +1082,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1090,16 +1099,16 @@
         <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" s="7">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1107,20 +1116,54 @@
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C24" s="7">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="7">
+        <v>75</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7">
+        <v>200</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E24" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
+  <autoFilter ref="A1:E26" xr:uid="{59229E94-6018-4A97-A06C-07B4D53DFD39}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>